<commit_message>
Product & Product content changes & Unit Test added
</commit_message>
<xml_diff>
--- a/FoodInfo.Service/OutsideFiles/ERRORS.xlsx
+++ b/FoodInfo.Service/OutsideFiles/ERRORS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\foodinfoservice\FoodInfo.Service\OutsideFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B766D360-D87E-4EDA-921C-5B8C137B93C4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D531D59-D87C-431E-B6C2-E1917F371D8D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="6930" xr2:uid="{3948AEF1-F3A6-46EE-A516-404323608713}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14490" windowHeight="4140" xr2:uid="{3948AEF1-F3A6-46EE-A516-404323608713}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>ErrorCode</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Please provide a language code.</t>
+  </si>
+  <si>
+    <t>CTN0002</t>
+  </si>
+  <si>
+    <t>There is a product content already exist.</t>
   </si>
 </sst>
 </file>
@@ -457,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{653980F5-A689-4090-8994-9EEDF8BE3653}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,9 +640,15 @@
       <c r="A12" t="s">
         <v>9</v>
       </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ERRORS (CreatedDate, IsDeleted, ErrorCode,ErrorMessage) Values ('2018-11-19',0,N'',N'')</v>
+        <v>INSERT INTO ERRORS (CreatedDate, IsDeleted, ErrorCode,ErrorMessage) Values ('2018-11-19',0,N'CTN0002',N'There is a product content already exist.')</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -686,5 +698,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>